<commit_message>
done w/ the chages
</commit_message>
<xml_diff>
--- a/src/test/resources/com/w2a/excel/testdata.xlsx
+++ b/src/test/resources/com/w2a/excel/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achal.Gupta\Documents\testing\testing-master\src\test\resources\com\w2a\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everythings AI\Documents\GitHub\test_framework\src\test\resources\com\w2a\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01154016-35FE-40CD-A923-C791798D0861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F11886-02BE-415C-AB0D-E9D0615FB213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Raman</t>
   </si>
@@ -56,16 +56,10 @@
     <t>Selenium@123</t>
   </si>
   <si>
-    <t>CreateAccountTest</t>
-  </si>
-  <si>
     <t>accountname</t>
   </si>
   <si>
-    <t>logintest</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>login</t>
   </si>
 </sst>
 </file>
@@ -394,15 +388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -410,19 +404,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -442,9 +428,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -455,7 +441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -486,14 +472,14 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>